<commit_message>
minor changes - unit tests (control) + engine mount design specs
</commit_message>
<xml_diff>
--- a/docs/Engine Mount.xlsx
+++ b/docs/Engine Mount.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2046BCE2-291D-FB4A-B002-64EE24758514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FCE152-CC52-7141-96B5-F1BAAE9E1ED2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EC1A70C0-1CE2-634C-8C72-C03DFFE023CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EC1A70C0-1CE2-634C-8C72-C03DFFE023CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Specs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Engine Mount Requirements</t>
   </si>
@@ -82,13 +83,55 @@
   </si>
   <si>
     <t>Avionics Comms and Ground Systems</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Mount Plate</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>curve radii = 3cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPR </t>
+  </si>
+  <si>
+    <t>LPR</t>
+  </si>
+  <si>
+    <t>PGR</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Edge Distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter </t>
+  </si>
+  <si>
+    <t>Edge Distance (From midpoint)</t>
+  </si>
+  <si>
+    <t>unit = cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +170,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,19 +219,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -178,6 +259,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6358F7C-FB0E-4C41-A947-951DD5879C51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6832600" y="177800"/>
+          <a:ext cx="7772400" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,84 +609,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D4E647-BC82-5347-9935-34A80E5872BF}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -615,4 +745,196 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251BBD76-9CC1-D543-A022-81B2FC2B8A95}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tiny changes everywhere - a shrinking problem
</commit_message>
<xml_diff>
--- a/docs/Engine Mount.xlsx
+++ b/docs/Engine Mount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FCE152-CC52-7141-96B5-F1BAAE9E1ED2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5719963E-C6D1-5D47-B393-15B3EA49CA80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{EC1A70C0-1CE2-634C-8C72-C03DFFE023CA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Engine Mount Requirements</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>unit = cm</t>
+  </si>
+  <si>
+    <t>Rough diagram</t>
   </si>
 </sst>
 </file>
@@ -749,10 +752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251BBD76-9CC1-D543-A022-81B2FC2B8A95}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,7 +861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -866,13 +869,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -880,7 +883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -888,21 +891,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -910,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -918,7 +925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -927,12 +934,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>